<commit_message>
Implement dialog to input new roommate Implement saving room and roommate into DB Hide Floating Button when go to Edit Room Fragment
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Story</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>I wan to send bills to other housemates</t>
+  </si>
+  <si>
+    <t>I want to validate input when adding new room</t>
+  </si>
+  <si>
+    <t>SPRINT 4</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -161,11 +170,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
@@ -187,8 +197,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{63B49E71-ABBD-43A3-B48B-08D52C13BABB}" name="Table2" displayName="Table2" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{A0CDD020-75B4-4813-BC2A-889BF5B03E89}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{63B49E71-ABBD-43A3-B48B-08D52C13BABB}" name="Table2" displayName="Table2" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{A0CDD020-75B4-4813-BC2A-889BF5B03E89}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E28D46FE-C7F6-419B-9C98-AEEE4FBD4CA2}" name="Sprint" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{660C2AB0-EB35-4438-A1ED-B8EF0E89CB30}" name="Story"/>
@@ -495,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F849A710-7EF0-4B30-9713-B8C9FD8D55B1}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,8 +536,8 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,8 +547,8 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,6 +614,17 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete view list of rooms
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Story</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>I want to get avatar for each housemate from the phone contact</t>
+  </si>
+  <si>
+    <t>I want to dispay room avatar as a combined image from roommates' avatars</t>
   </si>
 </sst>
 </file>
@@ -197,8 +203,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{63B49E71-ABBD-43A3-B48B-08D52C13BABB}" name="Table2" displayName="Table2" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10" xr:uid="{A0CDD020-75B4-4813-BC2A-889BF5B03E89}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{63B49E71-ABBD-43A3-B48B-08D52C13BABB}" name="Table2" displayName="Table2" ref="A1:C12" totalsRowShown="0">
+  <autoFilter ref="A1:C12" xr:uid="{A0CDD020-75B4-4813-BC2A-889BF5B03E89}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E28D46FE-C7F6-419B-9C98-AEEE4FBD4CA2}" name="Sprint" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{660C2AB0-EB35-4438-A1ED-B8EF0E89CB30}" name="Story"/>
@@ -505,16 +511,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F849A710-7EF0-4B30-9713-B8C9FD8D55B1}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="69.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -625,6 +631,28 @@
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
include update roommate feature
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -514,7 +514,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,8 +553,8 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,8 +564,8 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,8 +575,8 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
init templates for expense fragment
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Story</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>I want to dispay room avatar as a combined image from roommates' avatars</t>
+  </si>
+  <si>
+    <t>I want to copy over existing expenses to new month</t>
   </si>
 </sst>
 </file>
@@ -203,8 +206,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{63B49E71-ABBD-43A3-B48B-08D52C13BABB}" name="Table2" displayName="Table2" ref="A1:C12" totalsRowShown="0">
-  <autoFilter ref="A1:C12" xr:uid="{A0CDD020-75B4-4813-BC2A-889BF5B03E89}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{63B49E71-ABBD-43A3-B48B-08D52C13BABB}" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13" xr:uid="{A0CDD020-75B4-4813-BC2A-889BF5B03E89}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E28D46FE-C7F6-419B-9C98-AEEE4FBD4CA2}" name="Sprint" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{660C2AB0-EB35-4438-A1ED-B8EF0E89CB30}" name="Story"/>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F849A710-7EF0-4B30-9713-B8C9FD8D55B1}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +572,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
@@ -580,7 +583,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
@@ -591,7 +594,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
@@ -625,10 +628,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -639,7 +642,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -650,9 +653,20 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
include button to send bill
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443B8C85-DEF5-4AF9-B47F-8D11AF11DC32}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,12 +207,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0">
-  <autoFilter ref="A1:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Sprint" dataCellStyle="Good"/>
-    <tableColumn id="2" name="Story"/>
-    <tableColumn id="3" name="Status"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -501,28 +507,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="69.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -533,7 +539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -544,7 +550,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -555,7 +561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -566,7 +572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -577,7 +583,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -588,7 +594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -599,29 +605,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -632,7 +638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -643,7 +649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -654,7 +660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
implement feature to view previous month expenses
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443B8C85-DEF5-4AF9-B47F-8D11AF11DC32}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D6640A-6D47-42B7-B6AB-08C9F1FE1CD2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -518,7 +518,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,8 +623,8 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>6</v>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -634,8 +634,8 @@
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
implement feature to view bill for previous month
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D6640A-6D47-42B7-B6AB-08C9F1FE1CD2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED2BAD1-9A8C-4A25-ACBD-4BD616D388DD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Story</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>I want to copy over existing expenses to new month</t>
+  </si>
+  <si>
+    <t>I want to view fee and bill for previous months</t>
+  </si>
+  <si>
+    <t>I want to export and reimport DB</t>
   </si>
 </sst>
 </file>
@@ -207,8 +213,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0">
-  <autoFilter ref="A1:C13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,21 +638,21 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,7 +660,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -665,9 +671,31 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implement feature to copy fees from previous month to current month fix issue fee list not reloading after deleting fee
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED2BAD1-9A8C-4A25-ACBD-4BD616D388DD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BC3483-B0DF-4C62-8582-BF36156B8B9E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,8 +651,8 @@
       <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,8 +662,8 @@
       <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
implement restore DB feature
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BC3483-B0DF-4C62-8582-BF36156B8B9E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,12 +207,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="IN PROGRESS"/>
+        <filter val="NOT STARTED"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status"/>
+    <tableColumn id="1" name="Sprint" dataCellStyle="Good"/>
+    <tableColumn id="2" name="Story"/>
+    <tableColumn id="3" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -513,28 +514,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="69.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="69.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -545,7 +546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -556,7 +557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -567,7 +568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -578,7 +579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -589,7 +590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -600,7 +601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -611,8 +612,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
@@ -622,8 +623,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
@@ -633,8 +634,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
@@ -644,8 +645,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -655,30 +656,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
@@ -688,8 +689,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">

</xml_diff>

<commit_message>
display contact image for roommates in Edit Room screen
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CD5C64-7201-49A2-9D1C-51E9F7F4574D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>Story</t>
   </si>
@@ -91,12 +97,24 @@
   </si>
   <si>
     <t>I want to export and reimport DB</t>
+  </si>
+  <si>
+    <t>SPRINT 5</t>
+  </si>
+  <si>
+    <t>I want to include other options to send my bill rather than Whatsapp</t>
+  </si>
+  <si>
+    <t>I want to have place to store configurations: default message when sending bill, default app to send bill</t>
+  </si>
+  <si>
+    <t>I want to change app icon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,12 +198,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
@@ -207,19 +228,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="IN PROGRESS"/>
-        <filter val="NOT STARTED"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C18" totalsRowShown="0">
+  <autoFilter ref="A1:C18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Sprint" dataCellStyle="Good"/>
-    <tableColumn id="2" name="Story"/>
-    <tableColumn id="3" name="Status"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -514,28 +528,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="69.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -546,7 +560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -557,7 +571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -568,7 +582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -579,7 +593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -590,7 +604,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -601,7 +615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -612,7 +626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -623,7 +637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -634,7 +648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -645,7 +659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -656,7 +670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -667,29 +681,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -700,10 +714,44 @@
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
display roommate profile picture for fee share screen
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CD5C64-7201-49A2-9D1C-51E9F7F4574D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A10AFC7-B375-491D-8AE0-417132D6F75C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -539,7 +539,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,8 +699,8 @@
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>6</v>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -710,8 +710,8 @@
       <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>7</v>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
display room picture on monthly bill screens
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A10AFC7-B375-491D-8AE0-417132D6F75C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA112EF6-4CF0-4054-AF05-D71DBFCD487E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Story</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>I want to change app icon</t>
+  </si>
+  <si>
+    <t>I want to calculate some expense according to how many days housemates stay in house</t>
+  </si>
+  <si>
+    <t>I want to display expenses picture by type</t>
+  </si>
+  <si>
+    <t>SPRINT 6</t>
   </si>
 </sst>
 </file>
@@ -228,8 +237,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C18" totalsRowShown="0">
-  <autoFilter ref="A1:C18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
@@ -536,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,8 +719,8 @@
       <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>6</v>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,25 +734,47 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upgrade to Android Studio 3.1
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA112EF6-4CF0-4054-AF05-D71DBFCD487E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F95831-9A6C-4398-AC5D-BCC3705293F2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Story</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>SPRINT 6</t>
+  </si>
+  <si>
+    <t>I want to load profile picture asynchronous</t>
   </si>
 </sst>
 </file>
@@ -237,8 +240,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C20" totalsRowShown="0">
-  <autoFilter ref="A1:C20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C21" totalsRowShown="0">
+  <autoFilter ref="A1:C21" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
@@ -545,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +683,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
@@ -691,7 +694,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
@@ -702,7 +705,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
@@ -713,7 +716,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
@@ -724,7 +727,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B16" t="s">
@@ -735,7 +738,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
@@ -745,36 +748,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>26</v>
+      <c r="B18" t="s">
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
load higher quality contact photo
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692562DB-C53F-4747-A476-64150F290C01}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA937F4-8567-4079-9A1C-0372199F7209}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,8 +744,8 @@
       <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,8 +755,8 @@
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>7</v>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update new app logo
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA937F4-8567-4079-9A1C-0372199F7209}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EBE12C-CA1C-435B-8540-59A66F806F22}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +727,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B16" t="s">
@@ -738,7 +738,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
@@ -749,29 +749,29 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>6</v>
+      <c r="C18" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
+      <c r="C19" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
@@ -782,7 +782,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="5" t="s">

</xml_diff>

<commit_message>
implement static view for setting screen
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EBE12C-CA1C-435B-8540-59A66F806F22}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940B42B4-2193-4A36-BBFE-124A876FEF4D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Story</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>I want to load profile picture asynchronous</t>
+  </si>
+  <si>
+    <t>Fix request permission problem</t>
   </si>
 </sst>
 </file>
@@ -240,8 +243,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C21" totalsRowShown="0">
-  <autoFilter ref="A1:C21" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
@@ -548,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,21 +777,32 @@
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
-        <v>25</v>
+      <c r="B20" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save setting for deafult whastapp and default message when sending bill
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940B42B4-2193-4A36-BBFE-124A876FEF4D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,12 +237,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C22" totalsRowShown="0">
-  <autoFilter ref="A1:C22" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status"/>
+    <tableColumn id="1" name="Sprint" dataCellStyle="Good"/>
+    <tableColumn id="2" name="Story"/>
+    <tableColumn id="3" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -543,28 +537,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="69.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="69.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -575,7 +569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -586,7 +580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -597,7 +591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -608,7 +602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -619,7 +613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -630,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -641,7 +635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -652,7 +646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -663,7 +657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -674,7 +668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -685,7 +679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -696,7 +690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -707,7 +701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -718,7 +712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -729,7 +723,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -740,7 +734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -751,7 +745,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -762,40 +756,40 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
include new table for fee prepaid
</commit_message>
<xml_diff>
--- a/docs/Sprint Stories.xlsx
+++ b/docs/Sprint Stories.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkhoi\AndroidStudioProjects\SharedHouse\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA29A20-2F85-4098-A437-CE8B91CCCD85}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,12 +252,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C24" totalsRowShown="0">
-  <autoFilter ref="A1:C24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:C24" totalsRowShown="0">
+  <autoFilter ref="A1:C24" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Sprint" dataCellStyle="Good"/>
-    <tableColumn id="2" name="Story"/>
-    <tableColumn id="3" name="Status"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint" dataCellStyle="Good"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Story"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -546,28 +552,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="69.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -578,7 +584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -589,7 +595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -600,7 +606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -611,7 +617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -622,7 +628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -633,7 +639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -644,7 +650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -655,7 +661,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -666,7 +672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -677,7 +683,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -688,7 +694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -699,7 +705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -710,7 +716,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -721,7 +727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -732,7 +738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -743,7 +749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -754,7 +760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -765,7 +771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -776,7 +782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -787,7 +793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -798,29 +804,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>

</xml_diff>